<commit_message>
Respond to review comments
</commit_message>
<xml_diff>
--- a/verif/CV32E40P/VerificationPlan/base_instruction_set/CV32E40P_RV32M_Extension_Instructions.xlsx
+++ b/verif/CV32E40P/VerificationPlan/base_instruction_set/CV32E40P_RV32M_Extension_Instructions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\openhw\docs\core-v-docs.ArjanB_vplan_review\verif\CV32E40P\VerificationPlan\base_instruction_set\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{420A9C69-0786-4B65-9E50-C565A4109F8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD365129-FC6C-4358-9531-7DAE65D89864}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="High-level Feature" sheetId="1" r:id="rId1"/>
@@ -29,55 +29,28 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>Arjan Bink</author>
+    <author>tc={47A7F0D6-8B10-43D0-8302-EB9AF83D2A75}</author>
+    <author>tc={0E066E72-6E53-4B72-BEA1-0D3351A523A0}</author>
   </authors>
   <commentList>
-    <comment ref="E6" authorId="0" shapeId="0" xr:uid="{D820129E-B570-4DE1-A347-0F9C57AB06C0}">
+    <comment ref="E6" authorId="0" shapeId="0" xr:uid="{47A7F0D6-8B10-43D0-8302-EB9AF83D2A75}">
       <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Arjan Bink:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-CV32E40P does not 'fuse'</t>
-        </r>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    CV32E40P does not 'fuse'
+Reply:
+    Understood.  Feature has been stricken from the Vplan.</t>
       </text>
     </comment>
-    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{EB5E7A8C-9B89-43FA-B00C-55946B215412}">
+    <comment ref="B7" authorId="1" shapeId="0" xr:uid="{0E066E72-6E53-4B72-BEA1-0D3351A523A0}">
       <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Arjan Bink:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-The cycle counts for DIV, DIVU, REM, REMU are data dependent. We should trigger and check all possible cycle counts. There is an issue to get the expected cycle counts documented: https://github.com/openhwgroup/core-v-docs/issues/78</t>
-        </r>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    The cycle counts for DIV, DIVU, REM, REMU are data dependent. We should trigger and check all possible cycle counts. There is an issue to get the expected cycle counts documented: https://github.com/openhwgroup/core-v-docs/issues/78
+Reply:
+    Thanks for the reminder on this.  Rather than do that here, I propose to create a "micro-architectue" section of the Vplan and use that to verify all of the "Pipeline Details" chapter of the User Manual, including the Multi- and Single- cycle instructions table.</t>
       </text>
     </comment>
   </commentList>
@@ -783,14 +756,15 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
+      <strike/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="DejaVu Sans"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -809,12 +783,6 @@
         <bgColor rgb="FFCCFFFF"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -828,7 +796,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -862,18 +830,12 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -883,6 +845,16 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -967,6 +939,13 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Mike" id="{DDE7FACA-53EC-4778-BF47-0309545F7DDB}" userId="Mike" providerId="None"/>
+  <person displayName="Arjan Bink" id="{C7032DB6-46F7-4842-9B9D-157756460092}" userId="Arjan Bink" providerId="None"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1264,19 +1243,36 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="E6" personId="{C7032DB6-46F7-4842-9B9D-157756460092}" id="{47A7F0D6-8B10-43D0-8302-EB9AF83D2A75}">
+    <text>CV32E40P does not 'fuse'</text>
+  </threadedComment>
+  <threadedComment ref="E6" dT="2020-09-17T19:28:12.14" personId="{DDE7FACA-53EC-4778-BF47-0309545F7DDB}" id="{29699F40-7D62-4E12-8E85-A2EF17E0C64E}" parentId="{47A7F0D6-8B10-43D0-8302-EB9AF83D2A75}">
+    <text>Understood.  Feature has been stricken from the Vplan.</text>
+  </threadedComment>
+  <threadedComment ref="B7" personId="{C7032DB6-46F7-4842-9B9D-157756460092}" id="{0E066E72-6E53-4B72-BEA1-0D3351A523A0}">
+    <text>The cycle counts for DIV, DIVU, REM, REMU are data dependent. We should trigger and check all possible cycle counts. There is an issue to get the expected cycle counts documented: https://github.com/openhwgroup/core-v-docs/issues/78</text>
+  </threadedComment>
+  <threadedComment ref="B7" dT="2020-09-17T19:37:25.77" personId="{DDE7FACA-53EC-4778-BF47-0309545F7DDB}" id="{4C6D0E50-C0E9-4B84-B035-3C80EF041D4F}" parentId="{0E066E72-6E53-4B72-BEA1-0D3351A523A0}">
+    <text>Thanks for the reminder on this.  Rather than do that here, I propose to create a "micro-architectue" section of the Vplan and use that to verify all of the "Pipeline Details" chapter of the User Manual, including the Multi- and Single- cycle instructions table.</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ84"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="I15" sqref="I15"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="20.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="58.42578125" style="1" customWidth="1"/>
@@ -1315,18 +1311,18 @@
       <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="J1" s="15" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="5" customFormat="1" ht="71.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="19" t="s">
         <v>40</v>
       </c>
       <c r="C2" s="13" t="s">
@@ -1347,16 +1343,16 @@
       <c r="H2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="17" t="s">
+      <c r="I2" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="J2" s="17" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="5" customFormat="1" ht="85.5">
-      <c r="A3" s="21"/>
-      <c r="B3" s="21"/>
+      <c r="A3" s="19"/>
+      <c r="B3" s="19"/>
       <c r="C3" s="13" t="s">
         <v>44</v>
       </c>
@@ -1375,7 +1371,7 @@
       <c r="H3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="17" t="s">
+      <c r="I3" s="16" t="s">
         <v>73</v>
       </c>
       <c r="J3" s="1" t="s">
@@ -1383,8 +1379,8 @@
       </c>
     </row>
     <row r="4" spans="1:10" s="5" customFormat="1" ht="47.25">
-      <c r="A4" s="21"/>
-      <c r="B4" s="21"/>
+      <c r="A4" s="19"/>
+      <c r="B4" s="19"/>
       <c r="C4" s="13" t="s">
         <v>47</v>
       </c>
@@ -1403,7 +1399,7 @@
       <c r="H4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="17" t="s">
+      <c r="I4" s="16" t="s">
         <v>75</v>
       </c>
       <c r="J4" s="1" t="s">
@@ -1411,8 +1407,8 @@
       </c>
     </row>
     <row r="5" spans="1:10" s="5" customFormat="1" ht="85.5">
-      <c r="A5" s="21"/>
-      <c r="B5" s="21"/>
+      <c r="A5" s="19"/>
+      <c r="B5" s="19"/>
       <c r="C5" s="13" t="s">
         <v>50</v>
       </c>
@@ -1431,44 +1427,44 @@
       <c r="H5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="17" t="s">
+      <c r="I5" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="J5" s="18" t="s">
+      <c r="J5" s="17" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="5" customFormat="1" ht="42.75">
-      <c r="A6" s="21"/>
-      <c r="B6" s="21"/>
-      <c r="C6" s="15" t="s">
+      <c r="A6" s="19"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="I6" s="19"/>
+      <c r="I6" s="24"/>
       <c r="J6" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="5" customFormat="1" ht="171">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="19" t="s">
         <v>57</v>
       </c>
       <c r="C7" s="13" t="s">
@@ -1489,16 +1485,16 @@
       <c r="H7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="17" t="s">
+      <c r="I7" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="J7" s="18" t="s">
+      <c r="J7" s="17" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:10" s="5" customFormat="1" ht="156.75">
-      <c r="A8" s="21"/>
-      <c r="B8" s="21"/>
+      <c r="A8" s="19"/>
+      <c r="B8" s="19"/>
       <c r="C8" s="13" t="s">
         <v>61</v>
       </c>
@@ -1517,16 +1513,16 @@
       <c r="H8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="17" t="s">
+      <c r="I8" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="J8" s="18" t="s">
+      <c r="J8" s="17" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="5" customFormat="1" ht="85.5">
-      <c r="A9" s="21"/>
-      <c r="B9" s="21"/>
+      <c r="A9" s="19"/>
+      <c r="B9" s="19"/>
       <c r="C9" s="13" t="s">
         <v>64</v>
       </c>
@@ -1545,16 +1541,16 @@
       <c r="H9" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I9" s="17" t="s">
+      <c r="I9" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="J9" s="18" t="s">
+      <c r="J9" s="17" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:10" s="5" customFormat="1" ht="71.25">
-      <c r="A10" s="21"/>
-      <c r="B10" s="21"/>
+      <c r="A10" s="19"/>
+      <c r="B10" s="19"/>
       <c r="C10" s="13" t="s">
         <v>67</v>
       </c>
@@ -1573,25 +1569,25 @@
       <c r="H10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I10" s="17" t="s">
+      <c r="I10" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="J10" s="18" t="s">
+      <c r="J10" s="17" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="5" customFormat="1">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
     </row>
     <row r="12" spans="1:10" s="5" customFormat="1">
       <c r="A12" s="6"/>
@@ -2386,17 +2382,17 @@
       <c r="I83" s="6"/>
     </row>
     <row r="84" spans="1:9" s="8" customFormat="1">
-      <c r="A84" s="20" t="s">
+      <c r="A84" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B84" s="20"/>
-      <c r="C84" s="20"/>
-      <c r="D84" s="20"/>
-      <c r="E84" s="20"/>
-      <c r="F84" s="20"/>
-      <c r="G84" s="20"/>
-      <c r="H84" s="20"/>
-      <c r="I84" s="20"/>
+      <c r="B84" s="18"/>
+      <c r="C84" s="18"/>
+      <c r="D84" s="18"/>
+      <c r="E84" s="18"/>
+      <c r="F84" s="18"/>
+      <c r="G84" s="18"/>
+      <c r="H84" s="18"/>
+      <c r="I84" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -2408,8 +2404,8 @@
     <mergeCell ref="A11:I11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">

</xml_diff>